<commit_message>
Homing in on the big problem
</commit_message>
<xml_diff>
--- a/Geldautomat_ATM.xlsx
+++ b/Geldautomat_ATM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7610E78B-A7E3-48FA-8F5D-B3AB54B21B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295CEDCD-099E-4251-998A-E66A3EEAAB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{50C9C147-E925-4C04-99B8-FFE8930A841B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{50C9C147-E925-4C04-99B8-FFE8930A841B}"/>
   </bookViews>
   <sheets>
     <sheet name="Case DE" sheetId="4" r:id="rId1"/>
@@ -57,6 +57,7 @@
     <definedName name="_nz0">'Case EN'!$E$28:$E$37</definedName>
     <definedName name="_nz1">'Case EN'!$M$74:$M$83</definedName>
     <definedName name="_nz2">'Case EN'!$Q$97:$Q$106</definedName>
+    <definedName name="_tPivot">Banks!#REF!</definedName>
     <definedName name="IQ_DNTM" hidden="1">700000</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
@@ -144,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="215">
   <si>
     <t>Geldautomat</t>
   </si>
@@ -789,6 +790,12 @@
   </si>
   <si>
     <t>Difficult</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Quant</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1265,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1414,20 +1421,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1458,6 +1454,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed" wrapText="1"/>
@@ -2118,6 +2126,102 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49D4DA3F-2230-4C4C-BED6-889E08B5D9CF}" name="_tBank" displayName="_tBank" ref="C28:E98" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="C28:E98" xr:uid="{49D4DA3F-2230-4C4C-BED6-889E08B5D9CF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9CA12679-9DBA-43C0-8EFE-07F07C9489C5}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{CFE0F08D-3734-4924-B4BE-C38CA8C15771}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{16048123-E940-4294-964A-38F9FAAE3834}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{900FBF04-F0DD-47D8-8636-4AEC243A8A40}" name="_tTest" displayName="_tTest" ref="G28:I35" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="G28:I35" xr:uid="{900FBF04-F0DD-47D8-8636-4AEC243A8A40}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0D1C70D3-1213-46EE-BFFE-4AE81DA0C5A6}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{34EA618C-7022-4777-8007-D105E7C810A5}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{0842C844-3CDC-4157-83EC-E3BF52C4C2EA}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1E47546C-890C-46DA-8812-A7C1C26BD597}" name="_tP" displayName="_tP" ref="K28:M35" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="K28:M35" xr:uid="{1E47546C-890C-46DA-8812-A7C1C26BD597}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{892693C4-5AF4-404D-BC49-A2DCA887F4E3}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{3F1B599B-00F6-4875-BE08-73F59BCF3D8C}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{0F5E782B-F78C-42C4-9BED-A930A581A32C}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AB927C32-0C7D-4A02-B918-8931B88666E6}" name="Table7" displayName="Table7" ref="O28:Q35" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="O28:Q35" xr:uid="{AB927C32-0C7D-4A02-B918-8931B88666E6}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D02A7439-BD16-41BE-BCF5-6CC4A566462B}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{95357D46-10CE-4368-9B0F-B92042E3AB0B}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{7E6F2221-29C9-4F7A-B568-DD0326BE1603}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9218B3CE-8543-4018-95C7-C99A92DDB5B2}" name="_tS" displayName="_tS" ref="O37:Q44" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="O37:Q44" xr:uid="{9218B3CE-8543-4018-95C7-C99A92DDB5B2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DBBD0F1A-B87A-4C79-8E2E-8400432A7C5F}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{40CAF99F-86CA-4D7B-8FAE-272DDD6DD8A1}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{E1D2E569-0943-49F3-802F-366BEDCB6321}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FAC2B38D-EF66-45E1-BB0F-D634AC9644A3}" name="_tE" displayName="_tE" ref="K37:M44" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="K37:M44" xr:uid="{FAC2B38D-EF66-45E1-BB0F-D634AC9644A3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{72B0E0F8-3F93-4F91-867D-27F5A135EA5F}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{4488294F-FF23-47F4-AD59-6CC629398277}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{E01E2241-9A9D-49DF-ABF3-325062855D68}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{ACF9D383-2FF5-4C21-8C0A-1BE790430B1D}" name="_tBC" displayName="_tBC" ref="G37:I44" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="G37:I44" xr:uid="{ACF9D383-2FF5-4C21-8C0A-1BE790430B1D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{87315A26-C7EC-4F88-B265-C31EEB717ABE}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{50928503-4F39-45E7-AFD1-0D5B3175E167}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{3179809F-3170-483C-B50F-68455EB082AE}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A68C967C-4009-4CE3-BB93-DD36DD37BD9B}" name="_tI" displayName="_tI" ref="G46:I53" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="G46:I53" xr:uid="{A68C967C-4009-4CE3-BB93-DD36DD37BD9B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4A56FF31-7557-497A-BD85-B047CC187AE4}" name="Bank" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{40A2853E-4958-4265-9384-466B31469986}" name="Note" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{33902030-EB57-4EF3-9DBB-6149F1F2518C}" name="Quant" dataCellStyle="Standard 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2435,7 +2539,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="850" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="392" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2469,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A81AA6B-8E40-4088-895F-9744BA54F3C6}">
   <dimension ref="A2:O164"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4"/>
@@ -2498,18 +2602,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="60.75" customHeight="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="65"/>
     </row>
     <row r="3" spans="2:11" ht="21.75" customHeight="1">
       <c r="B3" s="1"/>
@@ -2522,46 +2626,46 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:11" ht="24" customHeight="1">
-      <c r="B4" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
     </row>
     <row r="5" spans="2:11" ht="67.5" customHeight="1">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="69" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="74"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="71"/>
     </row>
     <row r="6" spans="2:11" ht="25.5" customHeight="1">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="2:11" ht="15" customHeight="1">
       <c r="B7" s="4"/>
@@ -2620,13 +2724,13 @@
         <f>IF(ISBLANK(E11),0,IF(E11=Answers!E11,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
     </row>
     <row r="12" spans="2:11" ht="64.5" customHeight="1">
       <c r="B12" s="19" t="s">
@@ -2643,13 +2747,13 @@
         <f>IF(ISBLANK(E12),0,IF(E12=Answers!E12,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="2:11" ht="33.75" customHeight="1">
       <c r="B13" s="19" t="s">
@@ -2666,13 +2770,13 @@
         <f>IF(ISBLANK(E13),0,IF(E13=Answers!E13,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="61" t="s">
+      <c r="G13" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="2:11" ht="33.75" customHeight="1">
       <c r="B14" s="19" t="s">
@@ -2689,13 +2793,13 @@
         <f>IF(ISBLANK(E14),0,IF(E14=Answers!E14,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="61" t="s">
+      <c r="G14" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
     </row>
     <row r="15" spans="2:11" ht="21" customHeight="1">
       <c r="B15" s="4"/>
@@ -2729,12 +2833,12 @@
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
-      <c r="I17" s="65" t="str" cm="1">
+      <c r="I17" s="76" t="str" cm="1">
         <f t="array" ref="I17">SUMPRODUCT(--(F:F&gt;0),D:D)&amp;"/"&amp;SUM(D:D)</f>
         <v>0/370</v>
       </c>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
     </row>
     <row r="18" spans="2:11" ht="24.75" customHeight="1" thickBot="1">
       <c r="B18" s="27" t="s">
@@ -2744,23 +2848,23 @@
         <v>13</v>
       </c>
       <c r="D18" s="29"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1">
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1">
       <c r="B21" s="5" t="s">
@@ -3448,12 +3552,12 @@
       <c r="G70" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H70" s="62" t="s">
+      <c r="H70" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="I70" s="63"/>
-      <c r="J70" s="63"/>
-      <c r="K70" s="64"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="74"/>
+      <c r="K70" s="75"/>
     </row>
     <row r="71" spans="2:11" ht="15" customHeight="1">
       <c r="B71" s="1"/>
@@ -3882,18 +3986,18 @@
       <c r="G93" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H93" s="62" t="s">
+      <c r="H93" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="I93" s="63"/>
-      <c r="J93" s="63"/>
-      <c r="K93" s="64"/>
-      <c r="L93" s="62" t="s">
+      <c r="I93" s="74"/>
+      <c r="J93" s="74"/>
+      <c r="K93" s="75"/>
+      <c r="L93" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="M93" s="63"/>
-      <c r="N93" s="63"/>
-      <c r="O93" s="64"/>
+      <c r="M93" s="74"/>
+      <c r="N93" s="74"/>
+      <c r="O93" s="75"/>
     </row>
     <row r="94" spans="2:15" ht="15" customHeight="1">
       <c r="B94" s="1"/>
@@ -5320,18 +5424,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="L93:O93"/>
+    <mergeCell ref="I17:K20"/>
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B5:K5"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="L93:O93"/>
-    <mergeCell ref="I17:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5665,8 +5769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192E9B44-6F22-445A-9A18-8C4FDE921BA0}">
   <dimension ref="A2:Q171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView topLeftCell="E145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K158" sqref="K158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4"/>
@@ -5697,34 +5801,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="60.75" customHeight="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="65" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5739,80 +5843,80 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:11" ht="24" customHeight="1">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="I4" s="70" t="s">
+      <c r="I4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="J4" s="70" t="s">
+      <c r="J4" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="K4" s="71" t="s">
+      <c r="K4" s="68" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="67.5" customHeight="1">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="69" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="74"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="71"/>
     </row>
     <row r="6" spans="2:11" ht="25.5" customHeight="1">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="70" t="s">
+      <c r="I6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="K6" s="71" t="s">
+      <c r="K6" s="68" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5827,18 +5931,18 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="2:11" ht="15" customHeight="1">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
     </row>
     <row r="9" spans="2:11" ht="14.7" customHeight="1" thickBot="1">
       <c r="B9" s="5"/>
@@ -5884,19 +5988,19 @@
         <f>IF(ISBLANK(E11),0,IF(E11=Answers!E11,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="H11" s="75" t="s">
+      <c r="H11" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="I11" s="75" t="s">
+      <c r="I11" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="J11" s="75" t="s">
+      <c r="J11" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="72" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5915,19 +6019,19 @@
         <f>IF(ISBLANK(E12),0,IF(E12=Answers!E12,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="H12" s="61" t="s">
+      <c r="H12" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="K12" s="61" t="s">
+      <c r="K12" s="62" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5948,19 +6052,19 @@
         <f>IF(ISBLANK(E13),0,IF(E13=Answers!E13,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G13" s="61" t="s">
+      <c r="G13" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="H13" s="61" t="s">
+      <c r="H13" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="61" t="s">
+      <c r="I13" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="J13" s="61" t="s">
+      <c r="J13" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="K13" s="61" t="s">
+      <c r="K13" s="62" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5979,19 +6083,19 @@
         <f>IF(ISBLANK(E14),0,IF(E14=Answers!E14,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="61" t="s">
+      <c r="G14" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="H14" s="61" t="s">
+      <c r="H14" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="I14" s="61" t="s">
+      <c r="I14" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="J14" s="61" t="s">
+      <c r="J14" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="K14" s="61" t="s">
+      <c r="K14" s="62" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6028,12 +6132,12 @@
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
-      <c r="I17" s="65" t="str" cm="1">
+      <c r="I17" s="76" t="str" cm="1">
         <f t="array" ref="I17">SUMPRODUCT(--(F:F&gt;0),D:D)&amp;"/"&amp;SUM(D:D)</f>
         <v>180/370</v>
       </c>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
     </row>
     <row r="18" spans="2:11" ht="24.75" customHeight="1" thickBot="1">
       <c r="B18" s="27" t="s">
@@ -6043,23 +6147,23 @@
         <v>151</v>
       </c>
       <c r="D18" s="29"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1">
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>155</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1">
       <c r="B21" s="5" t="s">
@@ -6813,12 +6917,12 @@
       <c r="G70" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="H70" s="62" t="s">
+      <c r="H70" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="I70" s="63"/>
-      <c r="J70" s="63"/>
-      <c r="K70" s="64"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="74"/>
+      <c r="K70" s="75"/>
     </row>
     <row r="71" spans="2:16" ht="15" customHeight="1">
       <c r="B71" s="1"/>
@@ -7397,28 +7501,28 @@
       <c r="G93" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="H93" s="62" t="s">
+      <c r="H93" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="I93" s="63" t="s">
+      <c r="I93" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="J93" s="63" t="s">
+      <c r="J93" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="K93" s="64" t="s">
+      <c r="K93" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="L93" s="62" t="s">
+      <c r="L93" s="73" t="s">
         <v>210</v>
       </c>
-      <c r="M93" s="63" t="s">
+      <c r="M93" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="N93" s="63" t="s">
+      <c r="N93" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="O93" s="64" t="s">
+      <c r="O93" s="75" t="s">
         <v>139</v>
       </c>
     </row>
@@ -8788,22 +8892,22 @@
         <v>183</v>
       </c>
     </row>
-    <row r="145" spans="2:9" ht="14.7" customHeight="1">
+    <row r="145" spans="2:11" ht="14.7" customHeight="1">
       <c r="B145" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="146" spans="2:9" ht="14.7" customHeight="1">
+    <row r="146" spans="2:11" ht="14.7" customHeight="1">
       <c r="B146" s="5"/>
       <c r="C146" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="147" spans="2:9" ht="14.7" customHeight="1" thickBot="1">
+    <row r="147" spans="2:11" ht="14.7" customHeight="1" thickBot="1">
       <c r="B147" s="5"/>
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="2:9" ht="25.5" customHeight="1" thickBot="1">
+    <row r="148" spans="2:11" ht="25.5" customHeight="1" thickBot="1">
       <c r="B148" s="9" t="s">
         <v>141</v>
       </c>
@@ -8826,7 +8930,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="149" spans="2:9" ht="15" customHeight="1">
+    <row r="149" spans="2:11" ht="15" customHeight="1">
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
@@ -8834,7 +8938,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="2:9" ht="25.5" customHeight="1">
+    <row r="150" spans="2:11" ht="25.5" customHeight="1">
       <c r="B150" s="30" t="s">
         <v>181</v>
       </c>
@@ -8860,8 +8964,12 @@
       <c r="I150" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K150" s="1" cm="1">
+        <f t="array" ref="K150">INDEX(_xlfn.LET(_xlpm.nm, G150, _xlpm.no, _tTest[Note], _xlpm.qt, _tTest[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="2:11" ht="25.5" customHeight="1">
       <c r="B152" s="36">
         <v>51</v>
       </c>
@@ -8885,8 +8993,12 @@
       <c r="I152" s="34">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K152" s="61" cm="1">
+        <f t="array" ref="K152">INDEX(_xlfn.LET(_xlpm.nm, G152, _xlpm.no,_tP[Note], _xlpm.qt, _tP[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="2:11" ht="25.5" customHeight="1">
       <c r="B153" s="36">
         <v>52</v>
       </c>
@@ -8910,8 +9022,12 @@
       <c r="I153" s="34">
         <v>3</v>
       </c>
-    </row>
-    <row r="154" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K153" s="61" cm="1">
+        <f t="array" ref="K153">INDEX(_xlfn.LET(_xlpm.nm, G153, _xlpm.no, Table7[Note], _xlpm.qt, Table7[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="2:11" ht="25.5" customHeight="1">
       <c r="B154" s="36">
         <v>53</v>
       </c>
@@ -8935,8 +9051,12 @@
       <c r="I154" s="34">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K154" s="61" cm="1">
+        <f t="array" ref="K154">INDEX(_xlfn.LET(_xlpm.nm, G154, _xlpm.no, _tS[Note], _xlpm.qt, _tS[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="155" spans="2:11" ht="25.5" customHeight="1">
       <c r="B155" s="36">
         <v>54</v>
       </c>
@@ -8960,8 +9080,12 @@
       <c r="I155" s="34">
         <v>5</v>
       </c>
-    </row>
-    <row r="156" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K155" s="61" cm="1">
+        <f t="array" ref="K155">INDEX(_xlfn.LET(_xlpm.nm, G155, _xlpm.no, _tE[Note], _xlpm.qt, _tE[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="156" spans="2:11" ht="25.5" customHeight="1">
       <c r="B156" s="36">
         <v>55</v>
       </c>
@@ -8985,8 +9109,12 @@
       <c r="I156" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="157" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K156" s="61" cm="1">
+        <f t="array" ref="K156">INDEX(_xlfn.LET(_xlpm.nm, G156, _xlpm.no, _tBC[Note], _xlpm.qt, _tBC[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="2:11" ht="25.5" customHeight="1">
       <c r="B157" s="36">
         <v>56</v>
       </c>
@@ -9010,8 +9138,12 @@
       <c r="I157" s="34">
         <v>7</v>
       </c>
-    </row>
-    <row r="158" spans="2:9" ht="25.5" customHeight="1">
+      <c r="K157" s="61" cm="1">
+        <f t="array" ref="K157">INDEX(_xlfn.LET(_xlpm.nm, G157, _xlpm.no, _tI[Note], _xlpm.qt, _tI[Quant], _xlfn.REDUCE(_xlfn.VSTACK(_xlpm.nm, 0), _xlfn.SEQUENCE(7), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.am, INDEX(_xlpm.a, 1), _xlpm.nm, INDEX(_xlpm.a, 2), _xlpm.mx, INDEX(_xlpm.qt, _xlpm.v), _xlpm.div, INDEX(_xlpm.no, _xlpm.v), _xlpm.n_0, MIN(QUOTIENT(_xlpm.am, _xlpm.div), _xlpm.mx), _xlfn.VSTACK(INDEX(_xlpm.a, 1) - _xlpm.n_0 * _xlpm.div, INDEX(_xlpm.a, 2) + _xlpm.n_0))))),2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="158" spans="2:11" ht="25.5" customHeight="1">
       <c r="B158" s="36">
         <v>57</v>
       </c>
@@ -9036,7 +9168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:9" ht="25.5" customHeight="1">
+    <row r="159" spans="2:11" ht="25.5" customHeight="1">
       <c r="B159" s="36">
         <v>58</v>
       </c>
@@ -9061,7 +9193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="2:9" ht="25.5" customHeight="1">
+    <row r="160" spans="2:11" ht="25.5" customHeight="1">
       <c r="B160" s="36">
         <v>59</v>
       </c>
@@ -9715,8 +9847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF27E72-C0A8-423E-B550-B7E133FBE934}">
   <dimension ref="A2:O164"/>
   <sheetViews>
-    <sheetView topLeftCell="E69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4"/>
@@ -9744,18 +9876,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="60.75" customHeight="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="65"/>
     </row>
     <row r="3" spans="2:11" ht="21.75" customHeight="1">
       <c r="B3" s="1"/>
@@ -9768,46 +9900,46 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:11" ht="24" customHeight="1">
-      <c r="B4" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
     </row>
     <row r="5" spans="2:11" ht="67.5" customHeight="1">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="74"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="71"/>
     </row>
     <row r="6" spans="2:11" ht="25.5" customHeight="1">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="2:11" ht="15" customHeight="1">
       <c r="B7" s="4"/>
@@ -9865,13 +9997,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="18"/>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
     </row>
     <row r="12" spans="2:11" ht="64.5" customHeight="1">
       <c r="B12" s="19" t="s">
@@ -9887,13 +10019,13 @@
         <v>2204096</v>
       </c>
       <c r="F12" s="18"/>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="2:11" ht="33.75" customHeight="1">
       <c r="B13" s="19" t="s">
@@ -9909,13 +10041,13 @@
         <v>10004117235</v>
       </c>
       <c r="F13" s="18"/>
-      <c r="G13" s="61" t="s">
+      <c r="G13" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="2:11" ht="33.75" customHeight="1">
       <c r="B14" s="19" t="s">
@@ -9931,13 +10063,13 @@
         <v>949</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="61" t="s">
+      <c r="G14" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
     </row>
     <row r="15" spans="2:11" ht="21" customHeight="1">
       <c r="B15" s="4"/>
@@ -10631,12 +10763,12 @@
       <c r="G70" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H70" s="62" t="s">
+      <c r="H70" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="I70" s="63"/>
-      <c r="J70" s="63"/>
-      <c r="K70" s="64"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="74"/>
+      <c r="K70" s="75"/>
     </row>
     <row r="71" spans="2:11" ht="15" customHeight="1">
       <c r="B71" s="1"/>
@@ -11052,18 +11184,18 @@
       <c r="G93" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H93" s="62" t="s">
+      <c r="H93" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="I93" s="63"/>
-      <c r="J93" s="63"/>
-      <c r="K93" s="64"/>
-      <c r="L93" s="62" t="s">
+      <c r="I93" s="74"/>
+      <c r="J93" s="74"/>
+      <c r="K93" s="75"/>
+      <c r="L93" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="M93" s="63"/>
-      <c r="N93" s="63"/>
-      <c r="O93" s="64"/>
+      <c r="M93" s="74"/>
+      <c r="N93" s="74"/>
+      <c r="O93" s="75"/>
     </row>
     <row r="94" spans="2:15" ht="15" customHeight="1">
       <c r="B94" s="1"/>
@@ -11902,6 +12034,18 @@
     <row r="140" spans="2:9" ht="14.7" customHeight="1" thickBot="1">
       <c r="B140" s="5"/>
       <c r="C140" s="4"/>
+      <c r="G140" s="3" t="str">
+        <f>_xlfn.TRANSLATE(G141)</f>
+        <v>Amount</v>
+      </c>
+      <c r="H140" s="3" t="str">
+        <f t="shared" ref="H140:I140" si="0">_xlfn.TRANSLATE(H141)</f>
+        <v>Project</v>
+      </c>
+      <c r="I140" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Measure</v>
+      </c>
     </row>
     <row r="141" spans="2:9" ht="25.5" customHeight="1" thickBot="1">
       <c r="B141" s="9" t="s">
@@ -12440,19 +12584,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="L93:O93"/>
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B5:K5"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="L93:O93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -12939,21 +13084,21 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC71D1EF-0DAC-4349-8885-410BD14E743A}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A2:X25"/>
+  <dimension ref="A2:X98"/>
   <sheetViews>
-    <sheetView topLeftCell="L4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="C34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46:I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="25.8"/>
   <cols>
     <col min="1" max="1" width="21.109375" style="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="45" customWidth="1"/>
+    <col min="3" max="3" width="34" style="45" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" style="45" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" style="45" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" style="45" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.6640625" style="45" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.44140625" style="45" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.6640625" style="45" bestFit="1" customWidth="1"/>
@@ -13819,7 +13964,7 @@
         <v>3584</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" s="45" t="s">
         <v>53</v>
       </c>
@@ -13869,7 +14014,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" s="45" t="s">
         <v>53</v>
       </c>
@@ -13919,7 +14064,7 @@
         <v>4313</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="A19" s="45" t="s">
         <v>53</v>
       </c>
@@ -13969,7 +14114,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" s="45" t="s">
         <v>53</v>
       </c>
@@ -14019,7 +14164,7 @@
         <v>3698</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" s="45" t="s">
         <v>53</v>
       </c>
@@ -14069,7 +14214,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" s="45" t="s">
         <v>53</v>
       </c>
@@ -14119,7 +14264,7 @@
         <v>3379</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" s="45" t="s">
         <v>53</v>
       </c>
@@ -14169,7 +14314,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" s="45" t="s">
         <v>53</v>
       </c>
@@ -14219,7 +14364,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="C25" s="46">
         <f t="shared" ref="C25:P25" si="0">SUBTOTAL(109,C4:C24)</f>
         <v>5940107</v>
@@ -14277,11 +14422,1304 @@
         <v>40821</v>
       </c>
     </row>
+    <row r="28" spans="1:17">
+      <c r="C28" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="I28" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="K28" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="M28" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="O28" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="C29" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="45">
+        <v>100000</v>
+      </c>
+      <c r="E29" s="45">
+        <v>100</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="45">
+        <v>100</v>
+      </c>
+      <c r="I29" s="45">
+        <v>100</v>
+      </c>
+      <c r="K29" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L29" s="45">
+        <v>75462</v>
+      </c>
+      <c r="M29" s="45">
+        <v>972</v>
+      </c>
+      <c r="O29" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P29" s="45">
+        <v>83922</v>
+      </c>
+      <c r="Q29" s="45">
+        <v>3379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="C30" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="45">
+        <v>50000</v>
+      </c>
+      <c r="E30" s="45">
+        <v>100</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" s="45">
+        <v>50</v>
+      </c>
+      <c r="I30" s="45">
+        <v>100</v>
+      </c>
+      <c r="K30" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30" s="45">
+        <v>24310</v>
+      </c>
+      <c r="M30" s="45">
+        <v>2785</v>
+      </c>
+      <c r="O30" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P30" s="45">
+        <v>24169</v>
+      </c>
+      <c r="Q30" s="45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="C31" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="45">
+        <v>20000</v>
+      </c>
+      <c r="E31" s="45">
+        <v>100</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" s="45">
+        <v>20</v>
+      </c>
+      <c r="I31" s="45">
+        <v>100</v>
+      </c>
+      <c r="K31" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L31" s="45">
+        <v>4822</v>
+      </c>
+      <c r="M31" s="45">
+        <v>1801</v>
+      </c>
+      <c r="O31" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P31" s="45">
+        <v>4752</v>
+      </c>
+      <c r="Q31" s="45">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="C32" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="45">
+        <v>7500</v>
+      </c>
+      <c r="E32" s="45">
+        <v>100</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" s="45">
+        <v>10</v>
+      </c>
+      <c r="I32" s="45">
+        <v>100</v>
+      </c>
+      <c r="K32" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32" s="45">
+        <v>2724</v>
+      </c>
+      <c r="M32" s="45">
+        <v>1256</v>
+      </c>
+      <c r="O32" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P32" s="45">
+        <v>2784</v>
+      </c>
+      <c r="Q32" s="45">
+        <v>2772</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17">
+      <c r="C33" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="45">
+        <v>2250</v>
+      </c>
+      <c r="E33" s="45">
+        <v>100</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="45">
+        <v>5</v>
+      </c>
+      <c r="I33" s="45">
+        <v>100</v>
+      </c>
+      <c r="K33" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L33" s="45">
+        <v>199</v>
+      </c>
+      <c r="M33" s="45">
+        <v>3768</v>
+      </c>
+      <c r="O33" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P33" s="45">
+        <v>122</v>
+      </c>
+      <c r="Q33" s="45">
+        <v>3854</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17">
+      <c r="C34" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="45">
+        <v>25</v>
+      </c>
+      <c r="E34" s="45">
+        <v>100</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="45">
+        <v>2</v>
+      </c>
+      <c r="I34" s="45">
+        <v>100</v>
+      </c>
+      <c r="K34" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L34" s="45">
+        <v>45</v>
+      </c>
+      <c r="M34" s="45">
+        <v>1794</v>
+      </c>
+      <c r="O34" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P34" s="45">
+        <v>90</v>
+      </c>
+      <c r="Q34" s="45">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17">
+      <c r="C35" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="45">
+        <v>1</v>
+      </c>
+      <c r="E35" s="45">
+        <v>100</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="45">
+        <v>1</v>
+      </c>
+      <c r="I35" s="45">
+        <v>100</v>
+      </c>
+      <c r="K35" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="L35" s="45">
+        <v>1</v>
+      </c>
+      <c r="M35" s="45">
+        <v>1318</v>
+      </c>
+      <c r="O35" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P35" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="45">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17">
+      <c r="C36" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="45">
+        <v>62013</v>
+      </c>
+      <c r="E36" s="45">
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17">
+      <c r="C37" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="45">
+        <v>12152</v>
+      </c>
+      <c r="E37" s="45">
+        <v>3486</v>
+      </c>
+      <c r="G37" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="I37" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="K37" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="M37" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="O37" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="P37" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q37" s="45" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17">
+      <c r="C38" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="45">
+        <v>11241</v>
+      </c>
+      <c r="E38" s="45">
+        <v>2203</v>
+      </c>
+      <c r="G38" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="45">
+        <v>62013</v>
+      </c>
+      <c r="I38" s="45">
+        <v>3584</v>
+      </c>
+      <c r="K38" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" s="45">
+        <v>100000</v>
+      </c>
+      <c r="M38" s="45">
+        <v>100</v>
+      </c>
+      <c r="O38" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P38" s="45">
+        <v>90046</v>
+      </c>
+      <c r="Q38" s="45">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17">
+      <c r="C39" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="45">
+        <v>2850</v>
+      </c>
+      <c r="E39" s="45">
+        <v>3599</v>
+      </c>
+      <c r="G39" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="45">
+        <v>12152</v>
+      </c>
+      <c r="I39" s="45">
+        <v>3486</v>
+      </c>
+      <c r="K39" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" s="45">
+        <v>50000</v>
+      </c>
+      <c r="M39" s="45">
+        <v>100</v>
+      </c>
+      <c r="O39" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P39" s="45">
+        <v>13451</v>
+      </c>
+      <c r="Q39" s="45">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="40" spans="3:17">
+      <c r="C40" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="45">
+        <v>100</v>
+      </c>
+      <c r="E40" s="45">
+        <v>3635</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H40" s="45">
+        <v>11241</v>
+      </c>
+      <c r="I40" s="45">
+        <v>2203</v>
+      </c>
+      <c r="K40" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" s="45">
+        <v>20000</v>
+      </c>
+      <c r="M40" s="45">
+        <v>100</v>
+      </c>
+      <c r="O40" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P40" s="45">
+        <v>9278</v>
+      </c>
+      <c r="Q40" s="45">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17">
+      <c r="C41" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="45">
+        <v>94</v>
+      </c>
+      <c r="E41" s="45">
+        <v>2150</v>
+      </c>
+      <c r="G41" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" s="45">
+        <v>2850</v>
+      </c>
+      <c r="I41" s="45">
+        <v>3599</v>
+      </c>
+      <c r="K41" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="45">
+        <v>7500</v>
+      </c>
+      <c r="M41" s="45">
+        <v>100</v>
+      </c>
+      <c r="O41" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P41" s="45">
+        <v>3209</v>
+      </c>
+      <c r="Q41" s="45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17">
+      <c r="C42" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="45">
+        <v>1</v>
+      </c>
+      <c r="E42" s="45">
+        <v>1337</v>
+      </c>
+      <c r="G42" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H42" s="45">
+        <v>100</v>
+      </c>
+      <c r="I42" s="45">
+        <v>3635</v>
+      </c>
+      <c r="K42" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L42" s="45">
+        <v>2250</v>
+      </c>
+      <c r="M42" s="45">
+        <v>100</v>
+      </c>
+      <c r="O42" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P42" s="45">
+        <v>137</v>
+      </c>
+      <c r="Q42" s="45">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="43" spans="3:17">
+      <c r="C43" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="45">
+        <v>25398</v>
+      </c>
+      <c r="E43" s="45">
+        <v>321</v>
+      </c>
+      <c r="G43" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="45">
+        <v>94</v>
+      </c>
+      <c r="I43" s="45">
+        <v>2150</v>
+      </c>
+      <c r="K43" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" s="45">
+        <v>25</v>
+      </c>
+      <c r="M43" s="45">
+        <v>100</v>
+      </c>
+      <c r="O43" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P43" s="45">
+        <v>59</v>
+      </c>
+      <c r="Q43" s="45">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="44" spans="3:17">
+      <c r="C44" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="45">
+        <v>5414</v>
+      </c>
+      <c r="E44" s="45">
+        <v>3619</v>
+      </c>
+      <c r="G44" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" s="45">
+        <v>1</v>
+      </c>
+      <c r="I44" s="45">
+        <v>1337</v>
+      </c>
+      <c r="K44" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L44" s="45">
+        <v>1</v>
+      </c>
+      <c r="M44" s="45">
+        <v>100</v>
+      </c>
+      <c r="O44" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="P44" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="45">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="45" spans="3:17">
+      <c r="C45" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="45">
+        <v>4484</v>
+      </c>
+      <c r="E45" s="45">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="46" spans="3:17">
+      <c r="C46" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="45">
+        <v>3238</v>
+      </c>
+      <c r="E46" s="45">
+        <v>673</v>
+      </c>
+      <c r="G46" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="H46" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="I46" s="45" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17">
+      <c r="C47" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="45">
+        <v>130</v>
+      </c>
+      <c r="E47" s="45">
+        <v>2322</v>
+      </c>
+      <c r="G47" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H47" s="45">
+        <v>59042</v>
+      </c>
+      <c r="I47" s="45">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17">
+      <c r="C48" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="45">
+        <v>27</v>
+      </c>
+      <c r="E48" s="45">
+        <v>3235</v>
+      </c>
+      <c r="G48" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H48" s="45">
+        <v>34102</v>
+      </c>
+      <c r="I48" s="45">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9">
+      <c r="C49" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="45">
+        <v>1</v>
+      </c>
+      <c r="E49" s="45">
+        <v>3213</v>
+      </c>
+      <c r="G49" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H49" s="45">
+        <v>7985</v>
+      </c>
+      <c r="I49" s="45">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9">
+      <c r="C50" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="45">
+        <v>90046</v>
+      </c>
+      <c r="E50" s="45">
+        <v>4313</v>
+      </c>
+      <c r="G50" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="45">
+        <v>1213</v>
+      </c>
+      <c r="I50" s="45">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9">
+      <c r="C51" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="45">
+        <v>13451</v>
+      </c>
+      <c r="E51" s="45">
+        <v>2305</v>
+      </c>
+      <c r="G51" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H51" s="45">
+        <v>145</v>
+      </c>
+      <c r="I51" s="45">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9">
+      <c r="C52" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="45">
+        <v>9278</v>
+      </c>
+      <c r="E52" s="45">
+        <v>2168</v>
+      </c>
+      <c r="G52" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H52" s="45">
+        <v>50</v>
+      </c>
+      <c r="I52" s="45">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9">
+      <c r="C53" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="45">
+        <v>3209</v>
+      </c>
+      <c r="E53" s="45">
+        <v>119</v>
+      </c>
+      <c r="G53" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H53" s="45">
+        <v>1</v>
+      </c>
+      <c r="I53" s="45">
+        <v>3177</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9">
+      <c r="C54" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="45">
+        <v>137</v>
+      </c>
+      <c r="E54" s="45">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9">
+      <c r="C55" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="45">
+        <v>59</v>
+      </c>
+      <c r="E55" s="45">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9">
+      <c r="C56" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="45">
+        <v>1</v>
+      </c>
+      <c r="E56" s="45">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9">
+      <c r="C57" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="45">
+        <v>75462</v>
+      </c>
+      <c r="E57" s="45">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9">
+      <c r="C58" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" s="45">
+        <v>24310</v>
+      </c>
+      <c r="E58" s="45">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9">
+      <c r="C59" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="45">
+        <v>4822</v>
+      </c>
+      <c r="E59" s="45">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9">
+      <c r="C60" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="45">
+        <v>2724</v>
+      </c>
+      <c r="E60" s="45">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="61" spans="3:9">
+      <c r="C61" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="45">
+        <v>199</v>
+      </c>
+      <c r="E61" s="45">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9">
+      <c r="C62" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="45">
+        <v>45</v>
+      </c>
+      <c r="E62" s="45">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9">
+      <c r="C63" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="45">
+        <v>1</v>
+      </c>
+      <c r="E63" s="45">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="64" spans="3:9">
+      <c r="C64" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="45">
+        <v>54159</v>
+      </c>
+      <c r="E64" s="45">
+        <v>3698</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5">
+      <c r="C65" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D65" s="45">
+        <v>12111</v>
+      </c>
+      <c r="E65" s="45">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5">
+      <c r="C66" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" s="45">
+        <v>9313</v>
+      </c>
+      <c r="E66" s="45">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5">
+      <c r="C67" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" s="45">
+        <v>2427</v>
+      </c>
+      <c r="E67" s="45">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5">
+      <c r="C68" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D68" s="45">
+        <v>116</v>
+      </c>
+      <c r="E68" s="45">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5">
+      <c r="C69" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" s="45">
+        <v>71</v>
+      </c>
+      <c r="E69" s="45">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5">
+      <c r="C70" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="45">
+        <v>1</v>
+      </c>
+      <c r="E70" s="45">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5">
+      <c r="C71" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="45">
+        <v>39398</v>
+      </c>
+      <c r="E71" s="45">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5">
+      <c r="C72" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D72" s="45">
+        <v>22222</v>
+      </c>
+      <c r="E72" s="45">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5">
+      <c r="C73" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="45">
+        <v>9394</v>
+      </c>
+      <c r="E73" s="45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5">
+      <c r="C74" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="45">
+        <v>1469</v>
+      </c>
+      <c r="E74" s="45">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5">
+      <c r="C75" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D75" s="45">
+        <v>195</v>
+      </c>
+      <c r="E75" s="45">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5">
+      <c r="C76" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="45">
+        <v>100</v>
+      </c>
+      <c r="E76" s="45">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5">
+      <c r="C77" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" s="45">
+        <v>1</v>
+      </c>
+      <c r="E77" s="45">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5">
+      <c r="C78" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" s="45">
+        <v>83922</v>
+      </c>
+      <c r="E78" s="45">
+        <v>3379</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5">
+      <c r="C79" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="45">
+        <v>24169</v>
+      </c>
+      <c r="E79" s="45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5">
+      <c r="C80" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" s="45">
+        <v>4752</v>
+      </c>
+      <c r="E80" s="45">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5">
+      <c r="C81" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="45">
+        <v>2784</v>
+      </c>
+      <c r="E81" s="45">
+        <v>2772</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5">
+      <c r="C82" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D82" s="45">
+        <v>122</v>
+      </c>
+      <c r="E82" s="45">
+        <v>3854</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5">
+      <c r="C83" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D83" s="45">
+        <v>90</v>
+      </c>
+      <c r="E83" s="45">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5">
+      <c r="C84" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D84" s="45">
+        <v>1</v>
+      </c>
+      <c r="E84" s="45">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5">
+      <c r="C85" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="45">
+        <v>59042</v>
+      </c>
+      <c r="E85" s="45">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5">
+      <c r="C86" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" s="45">
+        <v>34102</v>
+      </c>
+      <c r="E86" s="45">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5">
+      <c r="C87" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D87" s="45">
+        <v>7985</v>
+      </c>
+      <c r="E87" s="45">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5">
+      <c r="C88" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D88" s="45">
+        <v>1213</v>
+      </c>
+      <c r="E88" s="45">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5">
+      <c r="C89" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="45">
+        <v>145</v>
+      </c>
+      <c r="E89" s="45">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5">
+      <c r="C90" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D90" s="45">
+        <v>50</v>
+      </c>
+      <c r="E90" s="45">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5">
+      <c r="C91" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D91" s="45">
+        <v>1</v>
+      </c>
+      <c r="E91" s="45">
+        <v>3177</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5">
+      <c r="C92" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D92" s="45">
+        <v>74884</v>
+      </c>
+      <c r="E92" s="45">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5">
+      <c r="C93" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D93" s="45">
+        <v>32415</v>
+      </c>
+      <c r="E93" s="45">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5">
+      <c r="C94" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D94" s="45">
+        <v>9040</v>
+      </c>
+      <c r="E94" s="45">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5">
+      <c r="C95" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D95" s="45">
+        <v>420</v>
+      </c>
+      <c r="E95" s="45">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5">
+      <c r="C96" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D96" s="45">
+        <v>137</v>
+      </c>
+      <c r="E96" s="45">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5">
+      <c r="C97" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D97" s="45">
+        <v>42</v>
+      </c>
+      <c r="E97" s="45">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5">
+      <c r="C98" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D98" s="45">
+        <v>1</v>
+      </c>
+      <c r="E98" s="45">
+        <v>3268</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>